<commit_message>
add h2 dependency for tests
</commit_message>
<xml_diff>
--- a/verifica_CPF.xlsx
+++ b/verifica_CPF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivola\OneDrive\Documents\Ivo\IBMEC\6° Período\Projeto Cloud\projeto_cloud_from_zero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11C96F1-533C-475E-BE44-D5E2893CAC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF7E3D-2D65-4AE4-BF17-211439806F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{5445A2DE-2620-4CDD-A09B-444AEFA508B7}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,35 +510,35 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K2" s="4">
         <f>SUM(A5:I5)</f>
-        <v>196</v>
+        <v>339</v>
       </c>
       <c r="L2" s="4">
         <f>MOD(K2,11)</f>
@@ -546,7 +546,7 @@
       </c>
       <c r="N2" s="5" t="str">
         <f>_xlfn.CONCAT(A8:C8,".",D8:F8,".",G8:I8,"-",J8:K8)</f>
-        <v>123.456.829-22</v>
+        <v>997.654.321-27</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -563,11 +563,11 @@
       <c r="I3" s="7"/>
       <c r="K3" s="4">
         <f>SUM(A11:J11)</f>
-        <v>240</v>
+        <v>389</v>
       </c>
       <c r="L3" s="4">
         <f>MOD(K3,11)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -602,19 +602,19 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ref="A5:I5" si="0">A2*A4</f>
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -622,11 +622,11 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -634,7 +634,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -659,19 +659,19 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" ref="A8:I8" si="1">A2</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
@@ -679,11 +679,11 @@
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f>IF(L2&lt;2,0,(11-L2))</f>
@@ -699,7 +699,7 @@
       </c>
       <c r="K8">
         <f>IF(L3&lt;2,0,11-L3)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -751,19 +751,19 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" ref="A11:J11" si="2">A8*A10</f>
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
@@ -771,11 +771,11 @@
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
@@ -783,7 +783,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>

</xml_diff>